<commit_message>
mudando o link no reenviar OS
</commit_message>
<xml_diff>
--- a/public/schools.xlsx
+++ b/public/schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanderson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanderson\Documents\CSDT-2\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD64225-FE83-4BBF-8B78-DE17652D5B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC13D4-8B08-4885-9B87-DCB673E8BA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="15180" xr2:uid="{67103AFA-85B7-437D-8CAA-1C23C31D43F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67103AFA-85B7-437D-8CAA-1C23C31D43F2}"/>
   </bookViews>
   <sheets>
     <sheet name="ESCOLAS TOTAL" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -6980,7 +6969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -7013,6 +7002,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12423,7 +12415,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B280B0FA-082A-4EC8-845C-634BB978D8E8}" name="Tabela5" displayName="Tabela5" ref="A1:G206" totalsRowShown="0">
-  <autoFilter ref="A1:G206" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A1:G206" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CRECHE MUNICIPAL PROFª JESUÍNA _x000a_FÁTIMA DE ANDRADE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{F8382116-AA6A-45EB-AEDA-E9A07B2D7C60}" name="NOME  DA  UNIDADE ESCOLAR" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{5331CCFC-BE7F-461E-BF9B-7A176943EA82}" name="INEP" dataDxfId="5">
@@ -12762,7 +12760,7 @@
   <dimension ref="A1:Y206"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -12818,7 +12816,7 @@
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
     </row>
-    <row r="2" spans="1:25" ht="45.75" customHeight="1">
+    <row r="2" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -12860,7 +12858,7 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
     </row>
-    <row r="3" spans="1:25" ht="45.75" customHeight="1">
+    <row r="3" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -12902,7 +12900,7 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:25" ht="45.75" customHeight="1">
+    <row r="4" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -12944,7 +12942,7 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:25" ht="45.75" customHeight="1">
+    <row r="5" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -12986,7 +12984,7 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25" ht="45.75" customHeight="1">
+    <row r="6" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
@@ -13028,7 +13026,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" ht="45.75" customHeight="1">
+    <row r="7" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -13070,7 +13068,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" ht="45.75" customHeight="1">
+    <row r="8" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -13112,7 +13110,7 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" ht="45.75" customHeight="1">
+    <row r="9" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -13154,7 +13152,7 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25" ht="45.75" customHeight="1">
+    <row r="10" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
@@ -13196,7 +13194,7 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="45.75" customHeight="1">
+    <row r="11" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>51</v>
       </c>
@@ -13238,7 +13236,7 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="45.75" customHeight="1">
+    <row r="12" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>56</v>
       </c>
@@ -13280,7 +13278,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="45.75" customHeight="1">
+    <row r="13" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>61</v>
       </c>
@@ -13322,7 +13320,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" ht="45.75" customHeight="1">
+    <row r="14" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -13364,7 +13362,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="45.75" customHeight="1">
+    <row r="15" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>71</v>
       </c>
@@ -13406,7 +13404,7 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="45.75" customHeight="1">
+    <row r="16" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>76</v>
       </c>
@@ -13448,7 +13446,7 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25" ht="45.75" customHeight="1">
+    <row r="17" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>81</v>
       </c>
@@ -13490,7 +13488,7 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" ht="45.75" customHeight="1">
+    <row r="18" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>86</v>
       </c>
@@ -13532,7 +13530,7 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" ht="45.75" customHeight="1">
+    <row r="19" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>91</v>
       </c>
@@ -13574,7 +13572,7 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" ht="45.75" customHeight="1">
+    <row r="20" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>96</v>
       </c>
@@ -13610,7 +13608,7 @@
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25" ht="45.75" customHeight="1">
+    <row r="21" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>98</v>
       </c>
@@ -13652,7 +13650,7 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25" ht="45.75" customHeight="1">
+    <row r="22" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>103</v>
       </c>
@@ -13694,7 +13692,7 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" ht="45.75" customHeight="1">
+    <row r="23" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>108</v>
       </c>
@@ -13736,7 +13734,7 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25" ht="45.75" customHeight="1">
+    <row r="24" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>113</v>
       </c>
@@ -13778,7 +13776,7 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="45.75" customHeight="1">
+    <row r="25" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>117</v>
       </c>
@@ -13820,7 +13818,7 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25" ht="45.75" customHeight="1">
+    <row r="26" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>122</v>
       </c>
@@ -13862,7 +13860,7 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25" ht="45.75" customHeight="1">
+    <row r="27" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>127</v>
       </c>
@@ -13904,7 +13902,7 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25" ht="45.75" customHeight="1">
+    <row r="28" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>132</v>
       </c>
@@ -13946,7 +13944,7 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25" ht="45.75" customHeight="1">
+    <row r="29" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>137</v>
       </c>
@@ -13988,7 +13986,7 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25" ht="45.75" customHeight="1">
+    <row r="30" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>142</v>
       </c>
@@ -14030,7 +14028,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25" ht="45.75" customHeight="1">
+    <row r="31" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>147</v>
       </c>
@@ -14072,7 +14070,7 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" ht="45.75" customHeight="1">
+    <row r="32" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A32" s="8" t="s">
         <v>152</v>
       </c>
@@ -14114,7 +14112,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25" ht="45.75" customHeight="1">
+    <row r="33" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>157</v>
       </c>
@@ -14156,7 +14154,7 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25" ht="45.75" customHeight="1">
+    <row r="34" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A34" s="8" t="s">
         <v>162</v>
       </c>
@@ -14198,7 +14196,7 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25" ht="45.75" customHeight="1">
+    <row r="35" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A35" s="8" t="s">
         <v>167</v>
       </c>
@@ -14240,7 +14238,7 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" spans="1:25" ht="45.75" customHeight="1">
+    <row r="36" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A36" s="8" t="s">
         <v>172</v>
       </c>
@@ -14282,7 +14280,7 @@
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" spans="1:25" ht="45.75" customHeight="1">
+    <row r="37" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>177</v>
       </c>
@@ -14324,7 +14322,7 @@
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" spans="1:25" ht="45.75" customHeight="1">
+    <row r="38" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A38" s="8" t="s">
         <v>182</v>
       </c>
@@ -14366,7 +14364,7 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" spans="1:25" ht="45.75" customHeight="1">
+    <row r="39" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A39" s="8" t="s">
         <v>187</v>
       </c>
@@ -14408,7 +14406,7 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
     </row>
-    <row r="40" spans="1:25" ht="45.75" customHeight="1">
+    <row r="40" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>192</v>
       </c>
@@ -14450,7 +14448,7 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
     </row>
-    <row r="41" spans="1:25" ht="45.75" customHeight="1">
+    <row r="41" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>197</v>
       </c>
@@ -14492,7 +14490,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
     </row>
-    <row r="42" spans="1:25" ht="45.75" customHeight="1">
+    <row r="42" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>202</v>
       </c>
@@ -14534,7 +14532,7 @@
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
     </row>
-    <row r="43" spans="1:25" ht="45.75" customHeight="1">
+    <row r="43" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A43" s="8" t="s">
         <v>207</v>
       </c>
@@ -14576,7 +14574,7 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
     </row>
-    <row r="44" spans="1:25" ht="45.75" customHeight="1">
+    <row r="44" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A44" s="8" t="s">
         <v>212</v>
       </c>
@@ -14618,7 +14616,7 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
     </row>
-    <row r="45" spans="1:25" ht="45.75" customHeight="1">
+    <row r="45" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A45" s="8" t="s">
         <v>217</v>
       </c>
@@ -14660,7 +14658,7 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
     </row>
-    <row r="46" spans="1:25" ht="45.75" customHeight="1">
+    <row r="46" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A46" s="8" t="s">
         <v>222</v>
       </c>
@@ -14702,7 +14700,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
     </row>
-    <row r="47" spans="1:25" ht="45.75" customHeight="1">
+    <row r="47" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A47" s="8" t="s">
         <v>227</v>
       </c>
@@ -14744,7 +14742,7 @@
       <c r="X47" s="5"/>
       <c r="Y47" s="5"/>
     </row>
-    <row r="48" spans="1:25" ht="45.75" customHeight="1">
+    <row r="48" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A48" s="8" t="s">
         <v>232</v>
       </c>
@@ -14786,7 +14784,7 @@
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
     </row>
-    <row r="49" spans="1:25" ht="45.75" customHeight="1">
+    <row r="49" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A49" s="8" t="s">
         <v>237</v>
       </c>
@@ -14828,7 +14826,7 @@
       <c r="X49" s="5"/>
       <c r="Y49" s="5"/>
     </row>
-    <row r="50" spans="1:25" ht="45.75" customHeight="1">
+    <row r="50" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A50" s="8" t="s">
         <v>242</v>
       </c>
@@ -14870,7 +14868,7 @@
       <c r="X50" s="5"/>
       <c r="Y50" s="5"/>
     </row>
-    <row r="51" spans="1:25" ht="45.75" customHeight="1">
+    <row r="51" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>247</v>
       </c>
@@ -14910,7 +14908,7 @@
       <c r="X51" s="5"/>
       <c r="Y51" s="5"/>
     </row>
-    <row r="52" spans="1:25" ht="45.75" customHeight="1">
+    <row r="52" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>249</v>
       </c>
@@ -14952,7 +14950,7 @@
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
     </row>
-    <row r="53" spans="1:25" ht="45.75" customHeight="1">
+    <row r="53" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>254</v>
       </c>
@@ -14994,7 +14992,7 @@
       <c r="X53" s="5"/>
       <c r="Y53" s="5"/>
     </row>
-    <row r="54" spans="1:25" ht="45.75" customHeight="1">
+    <row r="54" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>259</v>
       </c>
@@ -15036,7 +15034,7 @@
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
     </row>
-    <row r="55" spans="1:25" ht="45.75" customHeight="1">
+    <row r="55" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A55" s="8" t="s">
         <v>264</v>
       </c>
@@ -15078,7 +15076,7 @@
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
     </row>
-    <row r="56" spans="1:25" ht="45.75" customHeight="1">
+    <row r="56" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>269</v>
       </c>
@@ -15120,7 +15118,7 @@
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
     </row>
-    <row r="57" spans="1:25" ht="45.75" customHeight="1">
+    <row r="57" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>274</v>
       </c>
@@ -15162,7 +15160,7 @@
       <c r="X57" s="5"/>
       <c r="Y57" s="5"/>
     </row>
-    <row r="58" spans="1:25" ht="45.75" customHeight="1">
+    <row r="58" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A58" s="8" t="s">
         <v>279</v>
       </c>
@@ -15204,7 +15202,7 @@
       <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
     </row>
-    <row r="59" spans="1:25" ht="45.75" customHeight="1">
+    <row r="59" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A59" s="8" t="s">
         <v>284</v>
       </c>
@@ -15246,7 +15244,7 @@
       <c r="X59" s="5"/>
       <c r="Y59" s="5"/>
     </row>
-    <row r="60" spans="1:25" ht="45.75" customHeight="1">
+    <row r="60" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A60" s="8" t="s">
         <v>289</v>
       </c>
@@ -15288,7 +15286,7 @@
       <c r="X60" s="5"/>
       <c r="Y60" s="5"/>
     </row>
-    <row r="61" spans="1:25" ht="45.75" customHeight="1">
+    <row r="61" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>294</v>
       </c>
@@ -15330,7 +15328,7 @@
       <c r="X61" s="5"/>
       <c r="Y61" s="5"/>
     </row>
-    <row r="62" spans="1:25" ht="45.75" customHeight="1">
+    <row r="62" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A62" s="8" t="s">
         <v>299</v>
       </c>
@@ -15372,7 +15370,7 @@
       <c r="X62" s="5"/>
       <c r="Y62" s="5"/>
     </row>
-    <row r="63" spans="1:25" ht="45.75" customHeight="1">
+    <row r="63" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A63" s="8" t="s">
         <v>304</v>
       </c>
@@ -15414,7 +15412,7 @@
       <c r="X63" s="5"/>
       <c r="Y63" s="5"/>
     </row>
-    <row r="64" spans="1:25" ht="45.75" customHeight="1">
+    <row r="64" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A64" s="8" t="s">
         <v>309</v>
       </c>
@@ -15456,7 +15454,7 @@
       <c r="X64" s="5"/>
       <c r="Y64" s="5"/>
     </row>
-    <row r="65" spans="1:25" ht="45.75" customHeight="1">
+    <row r="65" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A65" s="8" t="s">
         <v>314</v>
       </c>
@@ -15498,7 +15496,7 @@
       <c r="X65" s="5"/>
       <c r="Y65" s="5"/>
     </row>
-    <row r="66" spans="1:25" ht="45.75" customHeight="1">
+    <row r="66" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A66" s="8" t="s">
         <v>319</v>
       </c>
@@ -15540,7 +15538,7 @@
       <c r="X66" s="5"/>
       <c r="Y66" s="5"/>
     </row>
-    <row r="67" spans="1:25" ht="45.75" customHeight="1">
+    <row r="67" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A67" s="8" t="s">
         <v>324</v>
       </c>
@@ -15582,7 +15580,7 @@
       <c r="X67" s="5"/>
       <c r="Y67" s="5"/>
     </row>
-    <row r="68" spans="1:25" ht="45.75" customHeight="1">
+    <row r="68" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A68" s="8" t="s">
         <v>329</v>
       </c>
@@ -15624,7 +15622,7 @@
       <c r="X68" s="5"/>
       <c r="Y68" s="5"/>
     </row>
-    <row r="69" spans="1:25" ht="45.75" customHeight="1">
+    <row r="69" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A69" s="8" t="s">
         <v>334</v>
       </c>
@@ -15666,7 +15664,7 @@
       <c r="X69" s="5"/>
       <c r="Y69" s="5"/>
     </row>
-    <row r="70" spans="1:25" ht="45.75" customHeight="1">
+    <row r="70" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A70" s="8" t="s">
         <v>339</v>
       </c>
@@ -15708,7 +15706,7 @@
       <c r="X70" s="5"/>
       <c r="Y70" s="5"/>
     </row>
-    <row r="71" spans="1:25" ht="45.75" customHeight="1">
+    <row r="71" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A71" s="8" t="s">
         <v>344</v>
       </c>
@@ -15750,7 +15748,7 @@
       <c r="X71" s="5"/>
       <c r="Y71" s="5"/>
     </row>
-    <row r="72" spans="1:25" ht="45.75" customHeight="1">
+    <row r="72" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A72" s="8" t="s">
         <v>349</v>
       </c>
@@ -15792,7 +15790,7 @@
       <c r="X72" s="5"/>
       <c r="Y72" s="5"/>
     </row>
-    <row r="73" spans="1:25" ht="45.75" customHeight="1">
+    <row r="73" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A73" s="8" t="s">
         <v>354</v>
       </c>
@@ -15834,7 +15832,7 @@
       <c r="X73" s="5"/>
       <c r="Y73" s="5"/>
     </row>
-    <row r="74" spans="1:25" ht="45.75" customHeight="1">
+    <row r="74" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A74" s="8" t="s">
         <v>358</v>
       </c>
@@ -15876,7 +15874,7 @@
       <c r="X74" s="5"/>
       <c r="Y74" s="5"/>
     </row>
-    <row r="75" spans="1:25" ht="45.75" customHeight="1">
+    <row r="75" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A75" s="8" t="s">
         <v>359</v>
       </c>
@@ -15918,7 +15916,7 @@
       <c r="X75" s="5"/>
       <c r="Y75" s="5"/>
     </row>
-    <row r="76" spans="1:25" ht="45.75" customHeight="1">
+    <row r="76" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A76" s="8" t="s">
         <v>364</v>
       </c>
@@ -15960,7 +15958,7 @@
       <c r="X76" s="5"/>
       <c r="Y76" s="5"/>
     </row>
-    <row r="77" spans="1:25" ht="45.75" customHeight="1">
+    <row r="77" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A77" s="8" t="s">
         <v>369</v>
       </c>
@@ -16002,7 +16000,7 @@
       <c r="X77" s="5"/>
       <c r="Y77" s="5"/>
     </row>
-    <row r="78" spans="1:25" ht="45.75" customHeight="1">
+    <row r="78" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A78" s="8" t="s">
         <v>374</v>
       </c>
@@ -16044,7 +16042,7 @@
       <c r="X78" s="5"/>
       <c r="Y78" s="5"/>
     </row>
-    <row r="79" spans="1:25" ht="45.75" customHeight="1">
+    <row r="79" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A79" s="8" t="s">
         <v>379</v>
       </c>
@@ -16086,7 +16084,7 @@
       <c r="X79" s="5"/>
       <c r="Y79" s="5"/>
     </row>
-    <row r="80" spans="1:25" ht="45.75" customHeight="1">
+    <row r="80" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A80" s="8" t="s">
         <v>384</v>
       </c>
@@ -16127,7 +16125,7 @@
       <c r="Y80" s="5"/>
     </row>
     <row r="81" spans="1:25" ht="45.75" customHeight="1">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="13" t="s">
         <v>385</v>
       </c>
       <c r="B81" s="7">
@@ -16168,7 +16166,7 @@
       <c r="X81" s="5"/>
       <c r="Y81" s="5"/>
     </row>
-    <row r="82" spans="1:25" ht="45.75" customHeight="1">
+    <row r="82" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A82" s="8" t="s">
         <v>390</v>
       </c>
@@ -16206,7 +16204,7 @@
       <c r="X82" s="5"/>
       <c r="Y82" s="5"/>
     </row>
-    <row r="83" spans="1:25" ht="45.75" customHeight="1">
+    <row r="83" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A83" s="8" t="s">
         <v>392</v>
       </c>
@@ -16248,7 +16246,7 @@
       <c r="X83" s="5"/>
       <c r="Y83" s="5"/>
     </row>
-    <row r="84" spans="1:25" ht="45.75" customHeight="1">
+    <row r="84" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A84" s="8" t="s">
         <v>397</v>
       </c>
@@ -16290,7 +16288,7 @@
       <c r="X84" s="5"/>
       <c r="Y84" s="5"/>
     </row>
-    <row r="85" spans="1:25" ht="45.75" customHeight="1">
+    <row r="85" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A85" s="8" t="s">
         <v>402</v>
       </c>
@@ -16332,7 +16330,7 @@
       <c r="X85" s="5"/>
       <c r="Y85" s="5"/>
     </row>
-    <row r="86" spans="1:25" ht="45.75" customHeight="1">
+    <row r="86" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A86" s="8" t="s">
         <v>407</v>
       </c>
@@ -16374,7 +16372,7 @@
       <c r="X86" s="5"/>
       <c r="Y86" s="5"/>
     </row>
-    <row r="87" spans="1:25" ht="45.75" customHeight="1">
+    <row r="87" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A87" s="8" t="s">
         <v>412</v>
       </c>
@@ -16416,7 +16414,7 @@
       <c r="X87" s="5"/>
       <c r="Y87" s="5"/>
     </row>
-    <row r="88" spans="1:25" ht="45.75" customHeight="1">
+    <row r="88" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A88" s="8" t="s">
         <v>417</v>
       </c>
@@ -16458,7 +16456,7 @@
       <c r="X88" s="5"/>
       <c r="Y88" s="5"/>
     </row>
-    <row r="89" spans="1:25" ht="45.75" customHeight="1">
+    <row r="89" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A89" s="8" t="s">
         <v>422</v>
       </c>
@@ -16500,7 +16498,7 @@
       <c r="X89" s="5"/>
       <c r="Y89" s="5"/>
     </row>
-    <row r="90" spans="1:25" ht="45.75" customHeight="1">
+    <row r="90" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A90" s="8" t="s">
         <v>427</v>
       </c>
@@ -16542,7 +16540,7 @@
       <c r="X90" s="5"/>
       <c r="Y90" s="5"/>
     </row>
-    <row r="91" spans="1:25" ht="45.75" customHeight="1">
+    <row r="91" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A91" s="8" t="s">
         <v>432</v>
       </c>
@@ -16584,7 +16582,7 @@
       <c r="X91" s="5"/>
       <c r="Y91" s="5"/>
     </row>
-    <row r="92" spans="1:25" ht="45.75" customHeight="1">
+    <row r="92" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A92" s="8" t="s">
         <v>437</v>
       </c>
@@ -16626,7 +16624,7 @@
       <c r="X92" s="5"/>
       <c r="Y92" s="5"/>
     </row>
-    <row r="93" spans="1:25" ht="45.75" customHeight="1">
+    <row r="93" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A93" s="8" t="s">
         <v>442</v>
       </c>
@@ -16668,7 +16666,7 @@
       <c r="X93" s="5"/>
       <c r="Y93" s="5"/>
     </row>
-    <row r="94" spans="1:25" ht="45.75" customHeight="1">
+    <row r="94" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A94" s="8" t="s">
         <v>447</v>
       </c>
@@ -16710,7 +16708,7 @@
       <c r="X94" s="5"/>
       <c r="Y94" s="5"/>
     </row>
-    <row r="95" spans="1:25" ht="45.75" customHeight="1">
+    <row r="95" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A95" s="8" t="s">
         <v>452</v>
       </c>
@@ -16752,7 +16750,7 @@
       <c r="X95" s="5"/>
       <c r="Y95" s="5"/>
     </row>
-    <row r="96" spans="1:25" ht="45.75" customHeight="1">
+    <row r="96" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A96" s="8" t="s">
         <v>457</v>
       </c>
@@ -16788,7 +16786,7 @@
       <c r="X96" s="5"/>
       <c r="Y96" s="5"/>
     </row>
-    <row r="97" spans="1:25" ht="45.75" customHeight="1">
+    <row r="97" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A97" s="8" t="s">
         <v>459</v>
       </c>
@@ -16830,7 +16828,7 @@
       <c r="X97" s="5"/>
       <c r="Y97" s="5"/>
     </row>
-    <row r="98" spans="1:25" ht="45.75" customHeight="1">
+    <row r="98" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A98" s="8" t="s">
         <v>464</v>
       </c>
@@ -16872,7 +16870,7 @@
       <c r="X98" s="5"/>
       <c r="Y98" s="5"/>
     </row>
-    <row r="99" spans="1:25" ht="45.75" customHeight="1">
+    <row r="99" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A99" s="8" t="s">
         <v>469</v>
       </c>
@@ -16914,7 +16912,7 @@
       <c r="X99" s="5"/>
       <c r="Y99" s="5"/>
     </row>
-    <row r="100" spans="1:25" ht="45.75" customHeight="1">
+    <row r="100" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A100" s="8" t="s">
         <v>474</v>
       </c>
@@ -16956,7 +16954,7 @@
       <c r="X100" s="5"/>
       <c r="Y100" s="5"/>
     </row>
-    <row r="101" spans="1:25" ht="45.75" customHeight="1">
+    <row r="101" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A101" s="8" t="s">
         <v>479</v>
       </c>
@@ -16998,7 +16996,7 @@
       <c r="X101" s="5"/>
       <c r="Y101" s="5"/>
     </row>
-    <row r="102" spans="1:25" ht="45.75" customHeight="1">
+    <row r="102" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A102" s="8" t="s">
         <v>484</v>
       </c>
@@ -17038,7 +17036,7 @@
       <c r="X102" s="5"/>
       <c r="Y102" s="5"/>
     </row>
-    <row r="103" spans="1:25" ht="45.75" customHeight="1">
+    <row r="103" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A103" s="8" t="s">
         <v>485</v>
       </c>
@@ -17080,7 +17078,7 @@
       <c r="X103" s="5"/>
       <c r="Y103" s="5"/>
     </row>
-    <row r="104" spans="1:25" ht="45.75" customHeight="1">
+    <row r="104" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A104" s="8" t="s">
         <v>490</v>
       </c>
@@ -17122,7 +17120,7 @@
       <c r="X104" s="5"/>
       <c r="Y104" s="5"/>
     </row>
-    <row r="105" spans="1:25" ht="45.75" customHeight="1">
+    <row r="105" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A105" s="8" t="s">
         <v>494</v>
       </c>
@@ -17164,7 +17162,7 @@
       <c r="X105" s="5"/>
       <c r="Y105" s="5"/>
     </row>
-    <row r="106" spans="1:25" ht="45.75" customHeight="1">
+    <row r="106" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A106" s="8" t="s">
         <v>499</v>
       </c>
@@ -17206,7 +17204,7 @@
       <c r="X106" s="5"/>
       <c r="Y106" s="5"/>
     </row>
-    <row r="107" spans="1:25" ht="45.75" customHeight="1">
+    <row r="107" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A107" s="8" t="s">
         <v>504</v>
       </c>
@@ -17248,7 +17246,7 @@
       <c r="X107" s="5"/>
       <c r="Y107" s="5"/>
     </row>
-    <row r="108" spans="1:25" ht="45.75" customHeight="1">
+    <row r="108" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A108" s="8" t="s">
         <v>509</v>
       </c>
@@ -17290,7 +17288,7 @@
       <c r="X108" s="5"/>
       <c r="Y108" s="5"/>
     </row>
-    <row r="109" spans="1:25" ht="45.75" customHeight="1">
+    <row r="109" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A109" s="8" t="s">
         <v>514</v>
       </c>
@@ -17332,7 +17330,7 @@
       <c r="X109" s="5"/>
       <c r="Y109" s="5"/>
     </row>
-    <row r="110" spans="1:25" ht="45.75" customHeight="1">
+    <row r="110" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A110" s="8" t="s">
         <v>519</v>
       </c>
@@ -17374,7 +17372,7 @@
       <c r="X110" s="5"/>
       <c r="Y110" s="5"/>
     </row>
-    <row r="111" spans="1:25" ht="45.75" customHeight="1">
+    <row r="111" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A111" s="8" t="s">
         <v>524</v>
       </c>
@@ -17416,7 +17414,7 @@
       <c r="X111" s="5"/>
       <c r="Y111" s="5"/>
     </row>
-    <row r="112" spans="1:25" ht="45.75" customHeight="1">
+    <row r="112" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A112" s="8" t="s">
         <v>529</v>
       </c>
@@ -17458,7 +17456,7 @@
       <c r="X112" s="5"/>
       <c r="Y112" s="5"/>
     </row>
-    <row r="113" spans="1:25" ht="45.75" customHeight="1">
+    <row r="113" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A113" s="8" t="s">
         <v>534</v>
       </c>
@@ -17500,7 +17498,7 @@
       <c r="X113" s="5"/>
       <c r="Y113" s="5"/>
     </row>
-    <row r="114" spans="1:25" ht="45.75" customHeight="1">
+    <row r="114" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A114" s="8" t="s">
         <v>538</v>
       </c>
@@ -17542,7 +17540,7 @@
       <c r="X114" s="5"/>
       <c r="Y114" s="5"/>
     </row>
-    <row r="115" spans="1:25" ht="45.75" customHeight="1">
+    <row r="115" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A115" s="8" t="s">
         <v>543</v>
       </c>
@@ -17584,7 +17582,7 @@
       <c r="X115" s="5"/>
       <c r="Y115" s="5"/>
     </row>
-    <row r="116" spans="1:25" ht="45.75" customHeight="1">
+    <row r="116" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A116" s="8" t="s">
         <v>548</v>
       </c>
@@ -17626,7 +17624,7 @@
       <c r="X116" s="5"/>
       <c r="Y116" s="5"/>
     </row>
-    <row r="117" spans="1:25" ht="45.75" customHeight="1">
+    <row r="117" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A117" s="8" t="s">
         <v>553</v>
       </c>
@@ -17668,7 +17666,7 @@
       <c r="X117" s="5"/>
       <c r="Y117" s="5"/>
     </row>
-    <row r="118" spans="1:25" ht="45.75" customHeight="1">
+    <row r="118" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A118" s="8" t="s">
         <v>558</v>
       </c>
@@ -17710,7 +17708,7 @@
       <c r="X118" s="5"/>
       <c r="Y118" s="5"/>
     </row>
-    <row r="119" spans="1:25" ht="45.75" customHeight="1">
+    <row r="119" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A119" s="8" t="s">
         <v>562</v>
       </c>
@@ -17752,7 +17750,7 @@
       <c r="X119" s="5"/>
       <c r="Y119" s="5"/>
     </row>
-    <row r="120" spans="1:25" ht="45.75" customHeight="1">
+    <row r="120" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A120" s="8" t="s">
         <v>567</v>
       </c>
@@ -17794,7 +17792,7 @@
       <c r="X120" s="5"/>
       <c r="Y120" s="5"/>
     </row>
-    <row r="121" spans="1:25" ht="45.75" customHeight="1">
+    <row r="121" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A121" s="8" t="s">
         <v>572</v>
       </c>
@@ -17836,7 +17834,7 @@
       <c r="X121" s="5"/>
       <c r="Y121" s="5"/>
     </row>
-    <row r="122" spans="1:25" ht="45.75" customHeight="1">
+    <row r="122" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A122" s="8" t="s">
         <v>577</v>
       </c>
@@ -17878,7 +17876,7 @@
       <c r="X122" s="5"/>
       <c r="Y122" s="5"/>
     </row>
-    <row r="123" spans="1:25" ht="45.75" customHeight="1">
+    <row r="123" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A123" s="8" t="s">
         <v>582</v>
       </c>
@@ -17920,7 +17918,7 @@
       <c r="X123" s="5"/>
       <c r="Y123" s="5"/>
     </row>
-    <row r="124" spans="1:25" ht="45.75" customHeight="1">
+    <row r="124" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A124" s="8" t="s">
         <v>587</v>
       </c>
@@ -17962,7 +17960,7 @@
       <c r="X124" s="5"/>
       <c r="Y124" s="5"/>
     </row>
-    <row r="125" spans="1:25" ht="45.75" customHeight="1">
+    <row r="125" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A125" s="8" t="s">
         <v>592</v>
       </c>
@@ -18004,7 +18002,7 @@
       <c r="X125" s="5"/>
       <c r="Y125" s="5"/>
     </row>
-    <row r="126" spans="1:25" ht="45.75" customHeight="1">
+    <row r="126" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A126" s="8" t="s">
         <v>597</v>
       </c>
@@ -18046,7 +18044,7 @@
       <c r="X126" s="5"/>
       <c r="Y126" s="5"/>
     </row>
-    <row r="127" spans="1:25" ht="45.75" customHeight="1">
+    <row r="127" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A127" s="8" t="s">
         <v>602</v>
       </c>
@@ -18088,7 +18086,7 @@
       <c r="X127" s="5"/>
       <c r="Y127" s="5"/>
     </row>
-    <row r="128" spans="1:25" ht="45.75" customHeight="1">
+    <row r="128" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A128" s="8" t="s">
         <v>607</v>
       </c>
@@ -18130,7 +18128,7 @@
       <c r="X128" s="5"/>
       <c r="Y128" s="5"/>
     </row>
-    <row r="129" spans="1:25" ht="45.75" customHeight="1">
+    <row r="129" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A129" s="8" t="s">
         <v>612</v>
       </c>
@@ -18172,7 +18170,7 @@
       <c r="X129" s="5"/>
       <c r="Y129" s="5"/>
     </row>
-    <row r="130" spans="1:25" ht="45.75" customHeight="1">
+    <row r="130" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A130" s="8" t="s">
         <v>617</v>
       </c>
@@ -18214,7 +18212,7 @@
       <c r="X130" s="5"/>
       <c r="Y130" s="5"/>
     </row>
-    <row r="131" spans="1:25" ht="45.75" customHeight="1">
+    <row r="131" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A131" s="8" t="s">
         <v>622</v>
       </c>
@@ -18256,7 +18254,7 @@
       <c r="X131" s="5"/>
       <c r="Y131" s="5"/>
     </row>
-    <row r="132" spans="1:25" ht="45.75" customHeight="1">
+    <row r="132" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A132" s="8" t="s">
         <v>627</v>
       </c>
@@ -18298,7 +18296,7 @@
       <c r="X132" s="5"/>
       <c r="Y132" s="5"/>
     </row>
-    <row r="133" spans="1:25" ht="45.75" customHeight="1">
+    <row r="133" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A133" s="8" t="s">
         <v>632</v>
       </c>
@@ -18340,7 +18338,7 @@
       <c r="X133" s="5"/>
       <c r="Y133" s="5"/>
     </row>
-    <row r="134" spans="1:25" ht="45.75" customHeight="1">
+    <row r="134" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A134" s="8" t="s">
         <v>637</v>
       </c>
@@ -18382,7 +18380,7 @@
       <c r="X134" s="5"/>
       <c r="Y134" s="5"/>
     </row>
-    <row r="135" spans="1:25" ht="45.75" customHeight="1">
+    <row r="135" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A135" s="8" t="s">
         <v>642</v>
       </c>
@@ -18424,7 +18422,7 @@
       <c r="X135" s="5"/>
       <c r="Y135" s="5"/>
     </row>
-    <row r="136" spans="1:25" ht="45.75" customHeight="1">
+    <row r="136" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A136" s="8" t="s">
         <v>647</v>
       </c>
@@ -18466,7 +18464,7 @@
       <c r="X136" s="5"/>
       <c r="Y136" s="5"/>
     </row>
-    <row r="137" spans="1:25" ht="45.75" customHeight="1">
+    <row r="137" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A137" s="8" t="s">
         <v>652</v>
       </c>
@@ -18508,7 +18506,7 @@
       <c r="X137" s="5"/>
       <c r="Y137" s="5"/>
     </row>
-    <row r="138" spans="1:25" ht="45.75" customHeight="1">
+    <row r="138" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A138" s="8" t="s">
         <v>657</v>
       </c>
@@ -18550,7 +18548,7 @@
       <c r="X138" s="5"/>
       <c r="Y138" s="5"/>
     </row>
-    <row r="139" spans="1:25" ht="45.75" customHeight="1">
+    <row r="139" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A139" s="8" t="s">
         <v>662</v>
       </c>
@@ -18592,7 +18590,7 @@
       <c r="X139" s="5"/>
       <c r="Y139" s="5"/>
     </row>
-    <row r="140" spans="1:25" ht="45.75" customHeight="1">
+    <row r="140" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A140" s="8" t="s">
         <v>667</v>
       </c>
@@ -18634,7 +18632,7 @@
       <c r="X140" s="5"/>
       <c r="Y140" s="5"/>
     </row>
-    <row r="141" spans="1:25" ht="45.75" customHeight="1">
+    <row r="141" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A141" s="8" t="s">
         <v>672</v>
       </c>
@@ -18676,7 +18674,7 @@
       <c r="X141" s="5"/>
       <c r="Y141" s="5"/>
     </row>
-    <row r="142" spans="1:25" ht="45.75" customHeight="1">
+    <row r="142" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A142" s="8" t="s">
         <v>677</v>
       </c>
@@ -18718,7 +18716,7 @@
       <c r="X142" s="5"/>
       <c r="Y142" s="5"/>
     </row>
-    <row r="143" spans="1:25" ht="45.75" customHeight="1">
+    <row r="143" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A143" s="8" t="s">
         <v>682</v>
       </c>
@@ -18760,7 +18758,7 @@
       <c r="X143" s="5"/>
       <c r="Y143" s="5"/>
     </row>
-    <row r="144" spans="1:25" ht="45.75" customHeight="1">
+    <row r="144" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A144" s="8" t="s">
         <v>687</v>
       </c>
@@ -18802,7 +18800,7 @@
       <c r="X144" s="5"/>
       <c r="Y144" s="5"/>
     </row>
-    <row r="145" spans="1:25" ht="45.75" customHeight="1">
+    <row r="145" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A145" s="8" t="s">
         <v>692</v>
       </c>
@@ -18844,7 +18842,7 @@
       <c r="X145" s="5"/>
       <c r="Y145" s="5"/>
     </row>
-    <row r="146" spans="1:25" ht="45.75" customHeight="1">
+    <row r="146" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A146" s="8" t="s">
         <v>697</v>
       </c>
@@ -18886,7 +18884,7 @@
       <c r="X146" s="5"/>
       <c r="Y146" s="5"/>
     </row>
-    <row r="147" spans="1:25" ht="45.75" customHeight="1">
+    <row r="147" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A147" s="8" t="s">
         <v>702</v>
       </c>
@@ -18928,7 +18926,7 @@
       <c r="X147" s="5"/>
       <c r="Y147" s="5"/>
     </row>
-    <row r="148" spans="1:25" ht="45.75" customHeight="1">
+    <row r="148" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A148" s="8" t="s">
         <v>707</v>
       </c>
@@ -18970,7 +18968,7 @@
       <c r="X148" s="5"/>
       <c r="Y148" s="5"/>
     </row>
-    <row r="149" spans="1:25" ht="45.75" customHeight="1">
+    <row r="149" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A149" s="8" t="s">
         <v>712</v>
       </c>
@@ -19012,7 +19010,7 @@
       <c r="X149" s="5"/>
       <c r="Y149" s="5"/>
     </row>
-    <row r="150" spans="1:25" ht="45.75" customHeight="1">
+    <row r="150" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A150" s="8" t="s">
         <v>717</v>
       </c>
@@ -19054,7 +19052,7 @@
       <c r="X150" s="5"/>
       <c r="Y150" s="5"/>
     </row>
-    <row r="151" spans="1:25" ht="45.75" customHeight="1">
+    <row r="151" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A151" s="8" t="s">
         <v>722</v>
       </c>
@@ -19096,7 +19094,7 @@
       <c r="X151" s="5"/>
       <c r="Y151" s="5"/>
     </row>
-    <row r="152" spans="1:25" ht="45.75" customHeight="1">
+    <row r="152" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A152" s="8" t="s">
         <v>727</v>
       </c>
@@ -19138,7 +19136,7 @@
       <c r="X152" s="5"/>
       <c r="Y152" s="5"/>
     </row>
-    <row r="153" spans="1:25" ht="45.75" customHeight="1">
+    <row r="153" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A153" s="8" t="s">
         <v>732</v>
       </c>
@@ -19180,7 +19178,7 @@
       <c r="X153" s="5"/>
       <c r="Y153" s="5"/>
     </row>
-    <row r="154" spans="1:25" ht="45.75" customHeight="1">
+    <row r="154" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A154" s="8" t="s">
         <v>737</v>
       </c>
@@ -19222,7 +19220,7 @@
       <c r="X154" s="5"/>
       <c r="Y154" s="5"/>
     </row>
-    <row r="155" spans="1:25" ht="45.75" customHeight="1">
+    <row r="155" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A155" s="8" t="s">
         <v>742</v>
       </c>
@@ -19264,7 +19262,7 @@
       <c r="X155" s="5"/>
       <c r="Y155" s="5"/>
     </row>
-    <row r="156" spans="1:25" ht="45.75" customHeight="1">
+    <row r="156" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A156" s="8" t="s">
         <v>747</v>
       </c>
@@ -19306,7 +19304,7 @@
       <c r="X156" s="5"/>
       <c r="Y156" s="5"/>
     </row>
-    <row r="157" spans="1:25" ht="45.75" customHeight="1">
+    <row r="157" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A157" s="8" t="s">
         <v>752</v>
       </c>
@@ -19348,7 +19346,7 @@
       <c r="X157" s="5"/>
       <c r="Y157" s="5"/>
     </row>
-    <row r="158" spans="1:25" ht="45.75" customHeight="1">
+    <row r="158" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A158" s="8" t="s">
         <v>757</v>
       </c>
@@ -19390,7 +19388,7 @@
       <c r="X158" s="5"/>
       <c r="Y158" s="5"/>
     </row>
-    <row r="159" spans="1:25" ht="45.75" customHeight="1">
+    <row r="159" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A159" s="8" t="s">
         <v>762</v>
       </c>
@@ -19432,7 +19430,7 @@
       <c r="X159" s="5"/>
       <c r="Y159" s="5"/>
     </row>
-    <row r="160" spans="1:25" ht="45.75" customHeight="1">
+    <row r="160" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A160" s="8" t="s">
         <v>767</v>
       </c>
@@ -19474,7 +19472,7 @@
       <c r="X160" s="5"/>
       <c r="Y160" s="5"/>
     </row>
-    <row r="161" spans="1:25" ht="45.75" customHeight="1">
+    <row r="161" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A161" s="8" t="s">
         <v>769</v>
       </c>
@@ -19516,7 +19514,7 @@
       <c r="X161" s="5"/>
       <c r="Y161" s="5"/>
     </row>
-    <row r="162" spans="1:25" ht="45.75" customHeight="1">
+    <row r="162" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A162" s="8" t="s">
         <v>774</v>
       </c>
@@ -19558,7 +19556,7 @@
       <c r="X162" s="5"/>
       <c r="Y162" s="5"/>
     </row>
-    <row r="163" spans="1:25" ht="45.75" customHeight="1">
+    <row r="163" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A163" s="8" t="s">
         <v>779</v>
       </c>
@@ -19600,7 +19598,7 @@
       <c r="X163" s="5"/>
       <c r="Y163" s="5"/>
     </row>
-    <row r="164" spans="1:25" ht="45.75" customHeight="1">
+    <row r="164" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A164" s="8" t="s">
         <v>784</v>
       </c>
@@ -19642,7 +19640,7 @@
       <c r="X164" s="5"/>
       <c r="Y164" s="5"/>
     </row>
-    <row r="165" spans="1:25" ht="45.75" customHeight="1">
+    <row r="165" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A165" s="8" t="s">
         <v>789</v>
       </c>
@@ -19684,7 +19682,7 @@
       <c r="X165" s="5"/>
       <c r="Y165" s="5"/>
     </row>
-    <row r="166" spans="1:25" ht="45.75" customHeight="1">
+    <row r="166" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A166" s="8" t="s">
         <v>794</v>
       </c>
@@ -19726,7 +19724,7 @@
       <c r="X166" s="5"/>
       <c r="Y166" s="5"/>
     </row>
-    <row r="167" spans="1:25" ht="45.75" customHeight="1">
+    <row r="167" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A167" s="8" t="s">
         <v>799</v>
       </c>
@@ -19768,7 +19766,7 @@
       <c r="X167" s="5"/>
       <c r="Y167" s="5"/>
     </row>
-    <row r="168" spans="1:25" ht="45.75" customHeight="1">
+    <row r="168" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A168" s="8" t="s">
         <v>804</v>
       </c>
@@ -19810,7 +19808,7 @@
       <c r="X168" s="5"/>
       <c r="Y168" s="5"/>
     </row>
-    <row r="169" spans="1:25" ht="45.75" customHeight="1">
+    <row r="169" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A169" s="8" t="s">
         <v>809</v>
       </c>
@@ -19852,7 +19850,7 @@
       <c r="X169" s="5"/>
       <c r="Y169" s="5"/>
     </row>
-    <row r="170" spans="1:25" ht="45.75" customHeight="1">
+    <row r="170" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A170" s="8" t="s">
         <v>814</v>
       </c>
@@ -19894,7 +19892,7 @@
       <c r="X170" s="5"/>
       <c r="Y170" s="5"/>
     </row>
-    <row r="171" spans="1:25" ht="45.75" customHeight="1">
+    <row r="171" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A171" s="8" t="s">
         <v>819</v>
       </c>
@@ -19936,7 +19934,7 @@
       <c r="X171" s="5"/>
       <c r="Y171" s="5"/>
     </row>
-    <row r="172" spans="1:25" ht="45.75" customHeight="1">
+    <row r="172" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A172" s="8" t="s">
         <v>824</v>
       </c>
@@ -19978,7 +19976,7 @@
       <c r="X172" s="5"/>
       <c r="Y172" s="5"/>
     </row>
-    <row r="173" spans="1:25" ht="45.75" customHeight="1">
+    <row r="173" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A173" s="8" t="s">
         <v>829</v>
       </c>
@@ -20020,7 +20018,7 @@
       <c r="X173" s="5"/>
       <c r="Y173" s="5"/>
     </row>
-    <row r="174" spans="1:25" ht="45.75" customHeight="1">
+    <row r="174" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A174" s="8" t="s">
         <v>834</v>
       </c>
@@ -20062,7 +20060,7 @@
       <c r="X174" s="5"/>
       <c r="Y174" s="5"/>
     </row>
-    <row r="175" spans="1:25" ht="45.75" customHeight="1">
+    <row r="175" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A175" s="8" t="s">
         <v>839</v>
       </c>
@@ -20104,7 +20102,7 @@
       <c r="X175" s="5"/>
       <c r="Y175" s="5"/>
     </row>
-    <row r="176" spans="1:25" ht="45.75" customHeight="1">
+    <row r="176" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A176" s="8" t="s">
         <v>844</v>
       </c>
@@ -20146,7 +20144,7 @@
       <c r="X176" s="5"/>
       <c r="Y176" s="5"/>
     </row>
-    <row r="177" spans="1:25" ht="45.75" customHeight="1">
+    <row r="177" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A177" s="8" t="s">
         <v>849</v>
       </c>
@@ -20188,7 +20186,7 @@
       <c r="X177" s="5"/>
       <c r="Y177" s="5"/>
     </row>
-    <row r="178" spans="1:25" ht="45.75" customHeight="1">
+    <row r="178" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A178" s="8" t="s">
         <v>854</v>
       </c>
@@ -20230,7 +20228,7 @@
       <c r="X178" s="5"/>
       <c r="Y178" s="5"/>
     </row>
-    <row r="179" spans="1:25" ht="45.75" customHeight="1">
+    <row r="179" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A179" s="8" t="s">
         <v>859</v>
       </c>
@@ -20272,7 +20270,7 @@
       <c r="X179" s="5"/>
       <c r="Y179" s="5"/>
     </row>
-    <row r="180" spans="1:25" ht="45.75" customHeight="1">
+    <row r="180" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A180" s="8" t="s">
         <v>864</v>
       </c>
@@ -20314,7 +20312,7 @@
       <c r="X180" s="5"/>
       <c r="Y180" s="5"/>
     </row>
-    <row r="181" spans="1:25" ht="45.75" customHeight="1">
+    <row r="181" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A181" s="8" t="s">
         <v>869</v>
       </c>
@@ -20356,7 +20354,7 @@
       <c r="X181" s="5"/>
       <c r="Y181" s="5"/>
     </row>
-    <row r="182" spans="1:25" ht="45.75" customHeight="1">
+    <row r="182" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A182" s="8" t="s">
         <v>874</v>
       </c>
@@ -20398,7 +20396,7 @@
       <c r="X182" s="5"/>
       <c r="Y182" s="5"/>
     </row>
-    <row r="183" spans="1:25" ht="45.75" customHeight="1">
+    <row r="183" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A183" s="8" t="s">
         <v>879</v>
       </c>
@@ -20440,7 +20438,7 @@
       <c r="X183" s="5"/>
       <c r="Y183" s="5"/>
     </row>
-    <row r="184" spans="1:25" ht="45.75" customHeight="1">
+    <row r="184" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A184" s="8" t="s">
         <v>884</v>
       </c>
@@ -20482,7 +20480,7 @@
       <c r="X184" s="5"/>
       <c r="Y184" s="5"/>
     </row>
-    <row r="185" spans="1:25" ht="45.75" customHeight="1">
+    <row r="185" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A185" s="8" t="s">
         <v>889</v>
       </c>
@@ -20524,7 +20522,7 @@
       <c r="X185" s="5"/>
       <c r="Y185" s="5"/>
     </row>
-    <row r="186" spans="1:25" ht="45.75" customHeight="1">
+    <row r="186" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A186" s="8" t="s">
         <v>894</v>
       </c>
@@ -20566,7 +20564,7 @@
       <c r="X186" s="5"/>
       <c r="Y186" s="5"/>
     </row>
-    <row r="187" spans="1:25" ht="45.75" customHeight="1">
+    <row r="187" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A187" s="8" t="s">
         <v>899</v>
       </c>
@@ -20608,7 +20606,7 @@
       <c r="X187" s="5"/>
       <c r="Y187" s="5"/>
     </row>
-    <row r="188" spans="1:25" ht="45.75" customHeight="1">
+    <row r="188" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A188" s="8" t="s">
         <v>904</v>
       </c>
@@ -20650,7 +20648,7 @@
       <c r="X188" s="5"/>
       <c r="Y188" s="5"/>
     </row>
-    <row r="189" spans="1:25" ht="45.75" customHeight="1">
+    <row r="189" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A189" s="8" t="s">
         <v>909</v>
       </c>
@@ -20692,7 +20690,7 @@
       <c r="X189" s="5"/>
       <c r="Y189" s="5"/>
     </row>
-    <row r="190" spans="1:25" ht="45.75" customHeight="1">
+    <row r="190" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A190" s="8" t="s">
         <v>914</v>
       </c>
@@ -20734,7 +20732,7 @@
       <c r="X190" s="5"/>
       <c r="Y190" s="5"/>
     </row>
-    <row r="191" spans="1:25" ht="45.75" customHeight="1">
+    <row r="191" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A191" s="8" t="s">
         <v>919</v>
       </c>
@@ -20776,7 +20774,7 @@
       <c r="X191" s="5"/>
       <c r="Y191" s="5"/>
     </row>
-    <row r="192" spans="1:25" ht="45.75" customHeight="1">
+    <row r="192" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A192" s="8" t="s">
         <v>924</v>
       </c>
@@ -20818,7 +20816,7 @@
       <c r="X192" s="5"/>
       <c r="Y192" s="5"/>
     </row>
-    <row r="193" spans="1:25" ht="45.75" customHeight="1">
+    <row r="193" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A193" s="8" t="s">
         <v>929</v>
       </c>
@@ -20860,7 +20858,7 @@
       <c r="X193" s="5"/>
       <c r="Y193" s="5"/>
     </row>
-    <row r="194" spans="1:25" ht="45.75" customHeight="1">
+    <row r="194" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A194" s="8" t="s">
         <v>934</v>
       </c>
@@ -20902,7 +20900,7 @@
       <c r="X194" s="5"/>
       <c r="Y194" s="5"/>
     </row>
-    <row r="195" spans="1:25" ht="45.75" customHeight="1">
+    <row r="195" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A195" s="8" t="s">
         <v>939</v>
       </c>
@@ -20944,7 +20942,7 @@
       <c r="X195" s="5"/>
       <c r="Y195" s="5"/>
     </row>
-    <row r="196" spans="1:25" ht="45.75" customHeight="1">
+    <row r="196" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A196" s="8" t="s">
         <v>944</v>
       </c>
@@ -20986,7 +20984,7 @@
       <c r="X196" s="5"/>
       <c r="Y196" s="5"/>
     </row>
-    <row r="197" spans="1:25" ht="45.75" customHeight="1">
+    <row r="197" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A197" s="8" t="s">
         <v>949</v>
       </c>
@@ -21028,7 +21026,7 @@
       <c r="X197" s="5"/>
       <c r="Y197" s="5"/>
     </row>
-    <row r="198" spans="1:25" ht="45.75" customHeight="1">
+    <row r="198" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A198" s="8" t="s">
         <v>954</v>
       </c>
@@ -21070,7 +21068,7 @@
       <c r="X198" s="5"/>
       <c r="Y198" s="5"/>
     </row>
-    <row r="199" spans="1:25" ht="45.75" customHeight="1">
+    <row r="199" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A199" s="8" t="s">
         <v>959</v>
       </c>
@@ -21112,7 +21110,7 @@
       <c r="X199" s="5"/>
       <c r="Y199" s="5"/>
     </row>
-    <row r="200" spans="1:25" ht="45.75" customHeight="1">
+    <row r="200" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A200" s="8" t="s">
         <v>964</v>
       </c>
@@ -21154,7 +21152,7 @@
       <c r="X200" s="5"/>
       <c r="Y200" s="5"/>
     </row>
-    <row r="201" spans="1:25" ht="45.75" customHeight="1">
+    <row r="201" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A201" s="8" t="s">
         <v>969</v>
       </c>
@@ -21196,7 +21194,7 @@
       <c r="X201" s="5"/>
       <c r="Y201" s="5"/>
     </row>
-    <row r="202" spans="1:25" ht="45.75" customHeight="1">
+    <row r="202" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A202" s="8" t="s">
         <v>974</v>
       </c>
@@ -21238,7 +21236,7 @@
       <c r="X202" s="5"/>
       <c r="Y202" s="5"/>
     </row>
-    <row r="203" spans="1:25" ht="45.75" customHeight="1">
+    <row r="203" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A203" s="8" t="s">
         <v>979</v>
       </c>
@@ -21280,7 +21278,7 @@
       <c r="X203" s="5"/>
       <c r="Y203" s="5"/>
     </row>
-    <row r="204" spans="1:25" ht="45.75" customHeight="1">
+    <row r="204" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A204" s="8" t="s">
         <v>980</v>
       </c>
@@ -21322,7 +21320,7 @@
       <c r="X204" s="5"/>
       <c r="Y204" s="5"/>
     </row>
-    <row r="205" spans="1:25" ht="45.75" customHeight="1">
+    <row r="205" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A205" s="8" t="s">
         <v>985</v>
       </c>
@@ -21364,7 +21362,7 @@
       <c r="X205" s="5"/>
       <c r="Y205" s="5"/>
     </row>
-    <row r="206" spans="1:25" ht="45.75" customHeight="1">
+    <row r="206" spans="1:25" ht="45.75" hidden="1" customHeight="1">
       <c r="A206" s="8" t="s">
         <v>990</v>
       </c>

</xml_diff>